<commit_message>
p2 e excel nba
</commit_message>
<xml_diff>
--- a/serie_a.xlsx
+++ b/serie_a.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ef875008baf77a9/Desktop/mate_sport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_AD4DB114E441178AC67DF45A5E13EC16693EDF26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{794C24D4-4813-4EDB-946A-804C707A6D13}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="11_AD4DB114E441178AC67DF45A5E13EC16693EDF26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61249E8A-9207-4BB4-BCBB-7098511DCDDD}"/>
   <bookViews>
-    <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Grafico1" sheetId="2" r:id="rId2"/>
+    <sheet name="Grafico2" sheetId="3" r:id="rId3"/>
+    <sheet name="Grafico3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -169,7 +172,563 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT" sz="1600" b="1"/>
+              <a:t>punti</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" sz="1600" b="1" baseline="0"/>
+              <a:t> / %goal per tiro</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.34678743961352659"/>
+          <c:y val="3.1712473572938688E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="1"/>
+            <c:backward val="1"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.57937198067632856"/>
+                  <c:y val="5.1892482784260847E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="it-IT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E787-403D-AF4D-11D055D95AD5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="12394687"/>
+        <c:axId val="172444383"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="12394687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="14"/>
+          <c:min val="2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="172444383"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="172444383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="12394687"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT" sz="1600" b="1"/>
+              <a:t>%goal per tiro / dist media tiri</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.28636072354990716"/>
+          <c:y val="2.448408534452606E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -225,8 +784,44 @@
             <c:trendlineType val="linear"/>
             <c:forward val="1"/>
             <c:backward val="1"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.876582861352866E-2"/>
+                  <c:y val="-0.43014461859633757"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="it-IT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -369,7 +964,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E5DD-46C2-846F-C2F96EDCE80A}"/>
+              <c16:uniqueId val="{00000002-1C1D-4AB0-8F0D-A3FF302AAF44}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -389,7 +984,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
-          <c:min val="12"/>
+          <c:min val="13"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -555,11 +1150,487 @@
       <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT" sz="1600" b="1"/>
+              <a:t>punti /dist media tiri</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="1"/>
+            <c:backward val="1"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.2669714916759323E-2"/>
+                  <c:y val="-0.60580233896248925"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="it-IT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>14.625228519195611</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.453382084095061</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.270566727605118</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.276051188299814</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.727605118829981</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.819012797074951</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.813528336380255</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.001828153564901</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.265082266910419</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.356489945155392</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16.819012797074951</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18.555758683729433</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.447897623400364</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16.361974405850088</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.813528336380255</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.9963436928702</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.82449725776965</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.367458866544787</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15.904936014625227</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16.910420475319924</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8F4E-49AA-8551-ED35DB742C99}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="180750335"/>
+        <c:axId val="181837551"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="180750335"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20"/>
+          <c:min val="13"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="181837551"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="181837551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="180750335"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
 </c:chartSpace>
 </file>
 
@@ -603,6 +1674,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1119,31 +2270,1091 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{E2393755-D4B4-42CE-ADBE-FED11AADAB99}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="109" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B61CD3CC-9A2A-4F0A-ACA1-6660EEAA7118}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="109" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{872F556C-7517-4157-872E-49055FDCF844}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9283817" cy="6061046"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CACA881-CBEA-A5C6-9084-7584019039C6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF70DF72-CFA9-1628-E77E-F3C7BBC29AD9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1156,8 +3367,78 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9283817" cy="6061046"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE3E660C-2721-19CC-9B65-8CC3E11D9E31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9283817" cy="6061046"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14496FBD-1C77-B8CB-FA3E-C93DCE1045AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1425,8 +3706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1753,6 +4034,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>